<commit_message>
Fix some logics in thongKe - Fix glitch display
</commit_message>
<xml_diff>
--- a/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
+++ b/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
@@ -73,10 +73,10 @@
     <t>Nhà Sách WhimsiBooks</t>
   </si>
   <si>
-    <t>Số HD: HD111223001</t>
-  </si>
-  <si>
-    <t>Ngày giờ: 21:55:42 - 11/12/2023</t>
+    <t>Số HD: HD121223001</t>
+  </si>
+  <si>
+    <t>Ngày giờ: 23:08:23 - 12/12/2023</t>
   </si>
   <si>
     <t>Khách hàng: Khách lẻ</t>

</xml_diff>

<commit_message>
Fix glitch: Khuyến mãi có hạn sử dụng, có lượt áp dụng, cập nhật trigger trừ số lượng khuyến mãi
</commit_message>
<xml_diff>
--- a/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
+++ b/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -73,22 +73,25 @@
     <t>Nhà Sách WhimsiBooks</t>
   </si>
   <si>
-    <t>Số HD: HD121223001</t>
-  </si>
-  <si>
-    <t>Ngày giờ: 23:08:23 - 12/12/2023</t>
+    <t>Số HD: HD131223005</t>
+  </si>
+  <si>
+    <t>Ngày giờ: 06:26:37 - 13/12/2023</t>
   </si>
   <si>
     <t>Khách hàng: Khách lẻ</t>
   </si>
   <si>
-    <t>NV bán hàng: Nguyễn Lê Nhật Huy</t>
-  </si>
-  <si>
-    <t>Vì tôi yêu cậu</t>
-  </si>
-  <si>
-    <t>194,400</t>
+    <t>NV bán hàng: Dương Thái Bảo</t>
+  </si>
+  <si>
+    <t>Mắt biếc</t>
+  </si>
+  <si>
+    <t>60,600</t>
+  </si>
+  <si>
+    <t>424,200</t>
   </si>
   <si>
     <t/>
@@ -100,13 +103,13 @@
     <t>Giảm giá:</t>
   </si>
   <si>
-    <t>19,440</t>
+    <t>84,840</t>
   </si>
   <si>
     <t>Tổng cộng:</t>
   </si>
   <si>
-    <t>174,960</t>
+    <t>339,360</t>
   </si>
   <si>
     <t>Tiền khách đưa:</t>
@@ -752,61 +755,61 @@
         <v>16</v>
       </c>
       <c r="C13" t="n" s="23">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="D13" t="s" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s" s="26">
         <v>17</v>
-      </c>
-      <c r="B14" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s" s="26">
-        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="s" s="25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s" s="25">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" t="s" s="25">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s" s="25">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s" s="25">
         <v>23</v>
-      </c>
-      <c r="D17" t="s" s="25">
-        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="s" s="25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s" s="25">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="27">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="21" s="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fix: Sửa lỗi trả hàng, cập nhật thông báo STMP Not Config yet
</commit_message>
<xml_diff>
--- a/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
+++ b/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -73,13 +73,13 @@
     <t>Nhà Sách WhimsiBooks</t>
   </si>
   <si>
-    <t>Số HD: HD131223003</t>
-  </si>
-  <si>
-    <t>Ngày giờ: 21:48:27 - 13/12/2023</t>
-  </si>
-  <si>
-    <t>Khách hàng: Khách lẻ</t>
+    <t>Số HD: HD141223005</t>
+  </si>
+  <si>
+    <t>Ngày giờ: 13:04:10 - 14/12/2023</t>
+  </si>
+  <si>
+    <t>Khách hàng: Nguyễn Thành Luân - KH0002</t>
   </si>
   <si>
     <t>NV bán hàng: Nguyễn Lê Nhật Huy</t>
@@ -91,34 +91,46 @@
     <t>60,600</t>
   </si>
   <si>
+    <t>303,000</t>
+  </si>
+  <si>
+    <t>Ngồi khóc trên cây</t>
+  </si>
+  <si>
+    <t>48,480</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>Tạm tính:</t>
   </si>
   <si>
+    <t>351,480</t>
+  </si>
+  <si>
     <t>Giảm giá:</t>
   </si>
   <si>
-    <t>1,818</t>
+    <t>30,300</t>
   </si>
   <si>
     <t>Tổng cộng:</t>
   </si>
   <si>
-    <t>58,782</t>
+    <t>321,180</t>
   </si>
   <si>
     <t>Tiền khách đưa:</t>
   </si>
   <si>
-    <t>60,000</t>
+    <t>350,000</t>
   </si>
   <si>
     <t>Tiền trả lại khách:</t>
   </si>
   <si>
-    <t>1,218</t>
+    <t>28,820</t>
   </si>
   <si>
     <t>Whimsibooks xin cảm ơn! Hẹn gặp lại quý khách!</t>
@@ -131,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -197,6 +209,10 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="20.0"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -253,7 +269,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -318,12 +334,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -755,65 +782,83 @@
         <v>16</v>
       </c>
       <c r="C13" t="n" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="D13" t="s" s="24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" ht="28.8" customHeight="true">
+      <c r="A14" t="n" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B14" t="s" s="26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" ht="28.8" customHeight="true">
+      <c r="B15" t="s" s="27">
+        <v>19</v>
+      </c>
+      <c r="C15" t="n" s="28">
         <v>1.0</v>
       </c>
-      <c r="D13" t="s" s="24">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s" s="26">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s" s="26">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" t="s" s="25">
+      <c r="D15" t="s" s="29">
         <v>19</v>
       </c>
-      <c r="D15" t="s" s="25">
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="31">
         <v>20</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="s" s="25">
+      <c r="B16" t="s" s="31">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s" s="31">
         <v>21</v>
       </c>
-      <c r="D16" t="s" s="25">
+      <c r="D16" t="s" s="31">
         <v>22</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="s" s="25">
+      <c r="C17" t="s" s="30">
         <v>23</v>
       </c>
-      <c r="D17" t="s" s="25">
+      <c r="D17" t="s" s="30">
         <v>24</v>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="s" s="25">
+      <c r="C18" t="s" s="30">
         <v>25</v>
       </c>
-      <c r="D18" t="s" s="25">
+      <c r="D18" t="s" s="30">
         <v>26</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="27">
+      <c r="C19" t="s" s="30">
         <v>27</v>
       </c>
+      <c r="D19" t="s" s="30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="s" s="30">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s" s="30">
+        <v>30</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="21" s="1" x14ac:dyDescent="0.35"/>
-    <row customFormat="1" customHeight="1" ht="28.95" r="22" s="1" x14ac:dyDescent="0.35"/>
+    <row r="22">
+      <c r="A22" t="s" s="32">
+        <v>31</v>
+      </c>
+    </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="23" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="24" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="25" s="1" x14ac:dyDescent="0.35"/>
@@ -834,7 +879,9 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.1" footer="0.1" header="0.1" left="0.1" right="0.1" top="0.4"/>

</xml_diff>

<commit_message>
fix: HoaDonTra feat - unknown problems
</commit_message>
<xml_diff>
--- a/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
+++ b/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -73,10 +73,10 @@
     <t>Nhà Sách WhimsiBooks</t>
   </si>
   <si>
-    <t>Số HD: HD120424002</t>
-  </si>
-  <si>
-    <t>Ngày giờ: 01:35:29 - 12/04/2024</t>
+    <t>Số HD: HD120424004</t>
+  </si>
+  <si>
+    <t>Ngày giờ: 16:14:02 - 12/04/2024</t>
   </si>
   <si>
     <t>Khách hàng: Khách lẻ</t>
@@ -97,13 +97,19 @@
     <t>87,360</t>
   </si>
   <si>
+    <t>Kéo</t>
+  </si>
+  <si>
+    <t>42,420</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>Tạm tính:</t>
   </si>
   <si>
-    <t>147,960</t>
+    <t>190,380</t>
   </si>
   <si>
     <t>Giảm giá:</t>
@@ -131,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -197,6 +203,10 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="20.0"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -257,7 +267,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -333,12 +343,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -795,60 +816,77 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="31">
-        <v>19</v>
+    <row r="16" ht="28.8" customHeight="true">
+      <c r="A16" t="n" s="30">
+        <v>3.0</v>
       </c>
       <c r="B16" t="s" s="31">
         <v>19</v>
       </c>
-      <c r="C16" t="s" s="31">
+    </row>
+    <row r="17" ht="28.8" customHeight="true">
+      <c r="B17" t="s" s="32">
         <v>20</v>
       </c>
-      <c r="D16" t="s" s="31">
+      <c r="C17" t="n" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="D17" t="s" s="34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="36">
         <v>21</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="s" s="30">
+      <c r="B18" t="s" s="36">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s" s="36">
         <v>22</v>
       </c>
-      <c r="D17" t="s" s="30">
+      <c r="D18" t="s" s="36">
         <v>23</v>
       </c>
     </row>
-    <row r="18">
-      <c r="C18" t="s" s="30">
+    <row r="19">
+      <c r="C19" t="s" s="35">
         <v>24</v>
       </c>
-      <c r="D18" t="s" s="30">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" t="s" s="30">
+      <c r="D19" t="s" s="35">
         <v>25</v>
       </c>
-      <c r="D19" t="s" s="30">
-        <v>21</v>
-      </c>
     </row>
     <row r="20">
-      <c r="C20" t="s" s="30">
+      <c r="C20" t="s" s="35">
         <v>26</v>
       </c>
-      <c r="D20" t="s" s="30">
+      <c r="D20" t="s" s="35">
         <v>23</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="28.95" r="21" s="1" x14ac:dyDescent="0.35"/>
+    <row r="21">
+      <c r="C21" t="s" s="35">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s" s="35">
+        <v>23</v>
+      </c>
+    </row>
     <row r="22">
-      <c r="A22" t="s" s="32">
-        <v>27</v>
+      <c r="C22" t="s" s="35">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s" s="35">
+        <v>25</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="23" s="1" x14ac:dyDescent="0.35"/>
-    <row customFormat="1" customHeight="1" ht="28.95" r="24" s="1" x14ac:dyDescent="0.35"/>
+    <row r="24">
+      <c r="A24" t="s" s="37">
+        <v>29</v>
+      </c>
+    </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="25" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="26" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="27" s="1" x14ac:dyDescent="0.35"/>
@@ -869,7 +907,9 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.1" footer="0.1" header="0.1" left="0.1" right="0.1" top="0.4"/>

</xml_diff>

<commit_message>
fix: The new bill same as the old bill (when use refund feat)
</commit_message>
<xml_diff>
--- a/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
+++ b/Nhom06_QuanLyWhimsiBooks/tempFile.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -73,10 +73,10 @@
     <t>Nhà Sách WhimsiBooks</t>
   </si>
   <si>
-    <t>Số HD: HD120424004</t>
-  </si>
-  <si>
-    <t>Ngày giờ: 16:14:02 - 12/04/2024</t>
+    <t>Số HD: HD120424008</t>
+  </si>
+  <si>
+    <t>Ngày giờ: 16:47:00 - 12/04/2024</t>
   </si>
   <si>
     <t>Khách hàng: Khách lẻ</t>
@@ -91,25 +91,22 @@
     <t>60,600</t>
   </si>
   <si>
+    <t>181,800</t>
+  </si>
+  <si>
     <t>BatMan</t>
   </si>
   <si>
     <t>87,360</t>
   </si>
   <si>
-    <t>Kéo</t>
-  </si>
-  <si>
-    <t>42,420</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>Tạm tính:</t>
   </si>
   <si>
-    <t>190,380</t>
+    <t>269,160</t>
   </si>
   <si>
     <t>Giảm giá:</t>
@@ -137,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -203,10 +200,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="20.0"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -267,7 +260,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -343,23 +336,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -791,10 +773,10 @@
         <v>16</v>
       </c>
       <c r="C13" t="n" s="23">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D13" t="s" s="24">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" ht="28.8" customHeight="true">
@@ -802,91 +784,74 @@
         <v>2.0</v>
       </c>
       <c r="B14" t="s" s="26">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" ht="28.8" customHeight="true">
       <c r="B15" t="s" s="27">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="n" s="28">
         <v>1.0</v>
       </c>
       <c r="D15" t="s" s="29">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" ht="28.8" customHeight="true">
-      <c r="A16" t="n" s="30">
-        <v>3.0</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="31">
+        <v>20</v>
       </c>
       <c r="B16" t="s" s="31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" ht="28.8" customHeight="true">
-      <c r="B17" t="s" s="32">
         <v>20</v>
       </c>
-      <c r="C17" t="n" s="33">
-        <v>1.0</v>
-      </c>
-      <c r="D17" t="s" s="34">
-        <v>20</v>
+      <c r="C16" t="s" s="31">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s" s="31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="s" s="30">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s" s="30">
+        <v>24</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s" s="36">
+      <c r="C18" t="s" s="30">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s" s="30">
         <v>22</v>
       </c>
-      <c r="D18" t="s" s="36">
-        <v>23</v>
-      </c>
     </row>
     <row r="19">
-      <c r="C19" t="s" s="35">
+      <c r="C19" t="s" s="30">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s" s="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="s" s="30">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s" s="30">
         <v>24</v>
       </c>
-      <c r="D19" t="s" s="35">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" t="s" s="35">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s" s="35">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" t="s" s="35">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s" s="35">
-        <v>23</v>
-      </c>
-    </row>
+    </row>
+    <row customFormat="1" customHeight="1" ht="28.95" r="21" s="1" x14ac:dyDescent="0.35"/>
     <row r="22">
-      <c r="C22" t="s" s="35">
+      <c r="A22" t="s" s="32">
         <v>28</v>
       </c>
-      <c r="D22" t="s" s="35">
-        <v>25</v>
-      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28.95" r="23" s="1" x14ac:dyDescent="0.35"/>
-    <row r="24">
-      <c r="A24" t="s" s="37">
-        <v>29</v>
-      </c>
-    </row>
+    <row customFormat="1" customHeight="1" ht="28.95" r="24" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="25" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="26" s="1" x14ac:dyDescent="0.35"/>
     <row customFormat="1" customHeight="1" ht="28.95" r="27" s="1" x14ac:dyDescent="0.35"/>
@@ -907,9 +872,7 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.1" footer="0.1" header="0.1" left="0.1" right="0.1" top="0.4"/>

</xml_diff>